<commit_message>
Updated risk list to include game related risks
</commit_message>
<xml_diff>
--- a/Documentation/Risk mangaement Log.xlsx
+++ b/Documentation/Risk mangaement Log.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PeacheyMacbook/Google Drive/Uni/Development-Project/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32900" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="32895" windowHeight="16875" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +13,9 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Risk_Area">[1]DropDown_Elements!$A$2:$A$30</definedName>
+    <definedName name="Risk_Area">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -193,6 +188,72 @@
   </si>
   <si>
     <t xml:space="preserve">Alternatively, the scope of the project would need to be changed to only use technologies that have been proven. </t>
+  </si>
+  <si>
+    <t>Game becomes boring</t>
+  </si>
+  <si>
+    <t>Risk the game will become stagnent for repeat users and there will be a large drop off in user activity and user staisfaction with the application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's Quiz requires a player base for users to compete against. If users are not playing the game the multiplayer aspect of the game will begin to fall apart. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High rate of uninstalls </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lack of new questions being submitted to the question pool. </t>
+  </si>
+  <si>
+    <t>The management team should systematically add questions to the question pool</t>
+  </si>
+  <si>
+    <t>Avoidance</t>
+  </si>
+  <si>
+    <t>Cheating</t>
+  </si>
+  <si>
+    <t>Potentially a player could devise a way to cheat and score above what they would have otherwise scored</t>
+  </si>
+  <si>
+    <t>Disproportionally high scroes being recorded in the global high score board</t>
+  </si>
+  <si>
+    <t>Dishonest player</t>
+  </si>
+  <si>
+    <t>Ban offending player and remove their score from the database</t>
+  </si>
+  <si>
+    <t>#006</t>
+  </si>
+  <si>
+    <t>Bad questions being submitted</t>
+  </si>
+  <si>
+    <t>There is no quality control measure in place to vet questions being submitted by the players. It is possible players could submit unreasonable questions, badly worded questions or querstions with incorrect answers</t>
+  </si>
+  <si>
+    <t>If players feel like they are not having a fair game then they will likely become disstatisfied with the application and stop playing</t>
+  </si>
+  <si>
+    <t>As a quiz game it is vital the questions being asked are of a high standard. If the standard of question being asked begins to fall it is very likely that players will become disstatisfied with the application and stop playing</t>
+  </si>
+  <si>
+    <t>High number of questions being down voted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor vetting </t>
+  </si>
+  <si>
+    <t>Contingency</t>
+  </si>
+  <si>
+    <t>Initally the plan is to use the question voting system to vet out bad questions after they have been submitted. If for example a new question was to receive 3 down votes in a row with no upvotes it could be removed</t>
+  </si>
+  <si>
+    <t>Introduce a manual vetting system that the Let's Quiz management team would have to maintain.</t>
   </si>
 </sst>
 </file>
@@ -202,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +328,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -504,7 +571,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -536,30 +603,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
@@ -607,6 +659,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -615,7 +670,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="55">
     <dxf>
       <fill>
         <patternFill>
@@ -640,6 +695,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="43"/>
         </patternFill>
       </fill>
@@ -647,6 +730,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="47"/>
         </patternFill>
       </fill>
@@ -661,6 +779,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="42"/>
         </patternFill>
       </fill>
@@ -689,6 +828,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="43"/>
         </patternFill>
       </fill>
@@ -703,6 +863,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="47"/>
         </patternFill>
       </fill>
@@ -735,8 +923,154 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="37"/>
+      <tableStyleElement type="headerRow" dxfId="36"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -749,110 +1083,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Instructions"/>
-      <sheetName val="Risk_Tracking_Log"/>
-      <sheetName val="DropDown_Elements"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Schedule</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Initial Costs</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Life-cycle Costs</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Technical Obsolescence</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Feasibility</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Reliability of Systems</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Dependencies/Interoperability</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Surety Considerations</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Future Procurements</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Project Management</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Overall Project Failure</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Organizational/Change Management</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Business</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Data/Information</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>Technology</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>Strategic</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>Security</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>Privacy</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>Project Resources</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1113,7 +1347,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1121,58 +1355,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="179" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
+    <col min="2" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" customWidth="1"/>
-    <col min="10" max="14" width="30.33203125" customWidth="1"/>
+    <col min="7" max="8" width="30.375" customWidth="1"/>
+    <col min="9" max="9" width="23.375" customWidth="1"/>
+    <col min="10" max="14" width="30.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="25" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="25" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:14" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1216,264 +1450,415 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="66" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:15" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="25" t="s">
         <v>44</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="25" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="55" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="25" t="s">
         <v>25</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="25" t="s">
         <v>49</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="55" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="30"/>
+      <c r="K10" s="25"/>
       <c r="L10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="N10" s="33" t="s">
+      <c r="N10" s="28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="13"/>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="F11" s="8" t="str">
         <f t="shared" ref="F11:F12" si="0">IF(OR(AND(B11&lt;&gt;"Closed",D11="High",E11="High"),AND(B11&lt;&gt;"Closed",D11="High",E11="Medium"),AND(B11&lt;&gt;"Closed",D11="Medium",E11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",D11="High",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Medium",E11="Medium"),AND(B11&lt;&gt;"Closed",D11="Low",E11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",D11="Medium",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Low",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Low",E11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
-        <v/>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
+        <v>Green</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+    <row r="12" spans="1:15" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="F12" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="18"/>
+        <f t="shared" ref="F12" si="1">IF(OR(AND(B12&lt;&gt;"Closed",D12="High",E12="High"),AND(B12&lt;&gt;"Closed",D12="High",E12="Medium"),AND(B12&lt;&gt;"Closed",D12="Medium",E12="High")),"Red",IF(OR(AND(B12&lt;&gt;"Closed",D12="High",E12="Low"),AND(B12&lt;&gt;"Closed",D12="Medium",E12="Medium"),AND(B12&lt;&gt;"Closed",D12="Low",E12="High")),"Yellow",IF(OR(AND(B12&lt;&gt;"Closed",D12="Medium",E12="Low"),AND(B12&lt;&gt;"Closed",D12="Low",E12="Low"),AND(B12&lt;&gt;"Closed",D12="Low",E12="Medium")),"Green",IF(B12="Closed","Closed",""))))</f>
+        <v>Green</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" s="13"/>
     </row>
-    <row r="15" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+    <row r="13" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="8" t="str">
+        <f t="shared" ref="F13" si="2">IF(OR(AND(B13&lt;&gt;"Closed",D13="High",E13="High"),AND(B13&lt;&gt;"Closed",D13="High",E13="Medium"),AND(B13&lt;&gt;"Closed",D13="Medium",E13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",D13="High",E13="Low"),AND(B13&lt;&gt;"Closed",D13="Medium",E13="Medium"),AND(B13&lt;&gt;"Closed",D13="Low",E13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",D13="Medium",E13="Low"),AND(B13&lt;&gt;"Closed",D13="Low",E13="Low"),AND(B13&lt;&gt;"Closed",D13="Low",E13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
+        <v>Yellow</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B7:D7 B11:C12 B8:B10">
-    <cfRule type="cellIs" dxfId="16" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="B7:D7 B8:B11">
+    <cfRule type="cellIs" dxfId="54" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="26" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M12">
-    <cfRule type="cellIs" dxfId="13" priority="10" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="F8 F10:F11">
+    <cfRule type="cellIs" dxfId="49" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"Red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="32" stopIfTrue="1" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:E11">
+    <cfRule type="cellIs" dxfId="46" priority="33" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8 F10:F12">
-    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Red"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Yellow"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Green"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:E12">
-    <cfRule type="cellIs" dxfId="8" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="35" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="22" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="23" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="19" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Critical"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:E12">
+    <cfRule type="cellIs" dxfId="23" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Critical"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="11" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:E13">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9 D8:E12 M11:M12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9 D8:E13">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L13">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B12 C11:C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B13">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I13">
       <formula1>Risk_Area</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New risk post changes to question genres
</commit_message>
<xml_diff>
--- a/Documentation/Risk mangaement Log.xlsx
+++ b/Documentation/Risk mangaement Log.xlsx
@@ -9,9 +9,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Risk_Area">#REF!</definedName>
   </definedNames>
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -254,6 +251,33 @@
   </si>
   <si>
     <t>Introduce a manual vetting system that the Let's Quiz management team would have to maintain.</t>
+  </si>
+  <si>
+    <t>#007</t>
+  </si>
+  <si>
+    <t>infringing on existing IP and copyright</t>
+  </si>
+  <si>
+    <t>With the change to our game from general trivia to sci fi and genre specific questions the risk of breaching copy right becomes quite high</t>
+  </si>
+  <si>
+    <t>Potentially we could be issued a cease and desist and be forced to remove all reference to the source material in question. If this was to happen to a popular category it will lead to customer dissatisfation, should it happen multiple times we would be left with very few catagories where questions could be asked</t>
+  </si>
+  <si>
+    <t>Gameplay, legal</t>
+  </si>
+  <si>
+    <t>Legal notice issued requesting Let's Quiz to cease and desist regarding references to a specific genre</t>
+  </si>
+  <si>
+    <t>Copy right infringment</t>
+  </si>
+  <si>
+    <t>Remove the offending questions</t>
+  </si>
+  <si>
+    <t>Initally if copy right is better understood it should become clearer whether or not Let's Quiz will be in breach</t>
   </si>
 </sst>
 </file>
@@ -670,7 +694,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="53">
     <dxf>
       <fill>
         <patternFill>
@@ -828,6 +852,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="47"/>
         </patternFill>
       </fill>
@@ -849,6 +894,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="43"/>
         </patternFill>
       </fill>
@@ -863,6 +929,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="42"/>
         </patternFill>
       </fill>
@@ -870,6 +957,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="43"/>
         </patternFill>
       </fill>
@@ -877,6 +978,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="45"/>
         </patternFill>
       </fill>
@@ -884,14 +992,35 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
         </patternFill>
       </fill>
     </dxf>
@@ -945,130 +1074,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="37"/>
-      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="wholeTable" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="51"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1077,19 +1087,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1347,7 +1344,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1357,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1594,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="8" t="str">
-        <f t="shared" ref="F11:F12" si="0">IF(OR(AND(B11&lt;&gt;"Closed",D11="High",E11="High"),AND(B11&lt;&gt;"Closed",D11="High",E11="Medium"),AND(B11&lt;&gt;"Closed",D11="Medium",E11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",D11="High",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Medium",E11="Medium"),AND(B11&lt;&gt;"Closed",D11="Low",E11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",D11="Medium",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Low",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Low",E11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
+        <f t="shared" ref="F11" si="0">IF(OR(AND(B11&lt;&gt;"Closed",D11="High",E11="High"),AND(B11&lt;&gt;"Closed",D11="High",E11="Medium"),AND(B11&lt;&gt;"Closed",D11="Medium",E11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",D11="High",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Medium",E11="Medium"),AND(B11&lt;&gt;"Closed",D11="Low",E11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",D11="Medium",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Low",E11="Low"),AND(B11&lt;&gt;"Closed",D11="Low",E11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
         <v>Green</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -1712,6 +1709,51 @@
       </c>
       <c r="N13" s="13" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="8" t="str">
+        <f t="shared" ref="F14" si="3">IF(OR(AND(B14&lt;&gt;"Closed",D14="High",E14="High"),AND(B14&lt;&gt;"Closed",D14="High",E14="Medium"),AND(B14&lt;&gt;"Closed",D14="Medium",E14="High")),"Red",IF(OR(AND(B14&lt;&gt;"Closed",D14="High",E14="Low"),AND(B14&lt;&gt;"Closed",D14="Medium",E14="Medium"),AND(B14&lt;&gt;"Closed",D14="Low",E14="High")),"Yellow",IF(OR(AND(B14&lt;&gt;"Closed",D14="Medium",E14="Low"),AND(B14&lt;&gt;"Closed",D14="Low",E14="Low"),AND(B14&lt;&gt;"Closed",D14="Low",E14="Medium")),"Green",IF(B14="Closed","Closed",""))))</f>
+        <v>Yellow</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,94 +1766,127 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7:D7 B8:B11">
-    <cfRule type="cellIs" dxfId="54" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="35" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8 F10:F11">
-    <cfRule type="cellIs" dxfId="49" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="39" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E11">
-    <cfRule type="cellIs" dxfId="46" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="42" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1">
-    <cfRule type="cellIs" dxfId="43" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="32" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="40" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="28" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="19" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="20" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="22" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="23" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:E12">
-    <cfRule type="cellIs" dxfId="23" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="25" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" dxfId="26" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Critical"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="23" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Green"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:E13">
+    <cfRule type="cellIs" dxfId="20" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
     <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -1822,7 +1897,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="F14">
     <cfRule type="cellIs" dxfId="11" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
@@ -1833,7 +1908,7 @@
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:E13">
+  <conditionalFormatting sqref="D14:E14">
     <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -1845,16 +1920,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9 D8:E13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9 D8:E14">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L14">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B14">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I14">
       <formula1>Risk_Area</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
small risk list update
</commit_message>
<xml_diff>
--- a/Documentation/Risk mangaement Log.xlsx
+++ b/Documentation/Risk mangaement Log.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PeacheyMacbook/Google Drive/Uni/Development-Project/Documentation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="32895" windowHeight="16875" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32900" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="Risk_Area">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -694,7 +699,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="44">
     <dxf>
       <fill>
         <patternFill>
@@ -726,70 +731,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1077,8 +1019,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="52"/>
-      <tableStyleElement type="headerRow" dxfId="51"/>
+      <tableStyleElement type="wholeTable" dxfId="43"/>
+      <tableStyleElement type="headerRow" dxfId="42"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1344,7 +1286,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1354,20 +1296,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="3" width="12.375" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="8" width="30.375" customWidth="1"/>
-    <col min="9" max="9" width="23.375" customWidth="1"/>
-    <col min="10" max="14" width="30.375" customWidth="1"/>
+    <col min="7" max="8" width="30.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
+    <col min="10" max="14" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1392,18 +1334,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1447,7 +1389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="66" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>18</v>
       </c>
@@ -1491,12 +1433,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="55" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>38</v>
@@ -1535,7 +1477,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="55" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
@@ -1577,7 +1519,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="44" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
@@ -1623,7 +1565,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="33" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>22</v>
       </c>
@@ -1666,7 +1608,7 @@
       </c>
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="55" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>64</v>
       </c>
@@ -1711,7 +1653,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="77" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>74</v>
       </c>
@@ -1756,166 +1698,166 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7:D7 B8:B11">
-    <cfRule type="cellIs" dxfId="50" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="35" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8 F10:F11">
-    <cfRule type="cellIs" dxfId="47" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E11">
-    <cfRule type="cellIs" dxfId="44" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="42" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="43" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1">
-    <cfRule type="cellIs" dxfId="41" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="32" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="38" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="28" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="35" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="20" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="32" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:E12">
-    <cfRule type="cellIs" dxfId="29" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="25" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="26" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="26" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="23" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:E13">
-    <cfRule type="cellIs" dxfId="20" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="11" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:E14">
-    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>